<commit_message>
geomap of area 1
still some error are occurring
- coludn't plot NaN values, so changed them to zero --> worked
- error occurs when trying to save, but figure is saved
- name error for last part of code
- did not yet implement f"
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_count.xlsx
+++ b/_CLUSTER/groups_count.xlsx
@@ -1,81 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_CLUSTER\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF04CF56-DCC7-4202-BDD0-307570007334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>area1</t>
-  </si>
-  <si>
-    <t>area2</t>
-  </si>
-  <si>
-    <t>area3</t>
-  </si>
-  <si>
-    <t>area4</t>
-  </si>
-  <si>
-    <t>area5</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,47 +46,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -418,193 +353,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>area1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>area2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>area3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>area4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>area5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
+        <v>543</v>
+      </c>
+      <c r="C2" t="n">
+        <v>384</v>
+      </c>
+      <c r="D2" t="n">
+        <v>416</v>
+      </c>
+      <c r="E2" t="n">
+        <v>213</v>
+      </c>
+      <c r="F2" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="n">
+        <v>805</v>
+      </c>
+      <c r="C3" t="n">
+        <v>563</v>
+      </c>
+      <c r="D3" t="n">
+        <v>531</v>
+      </c>
+      <c r="E3" t="n">
+        <v>174</v>
+      </c>
+      <c r="F3" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>543</v>
-      </c>
-      <c r="C2">
-        <v>384</v>
-      </c>
-      <c r="D2">
-        <v>416</v>
-      </c>
-      <c r="E2">
-        <v>208</v>
-      </c>
-      <c r="F2">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>805</v>
-      </c>
-      <c r="C3">
-        <v>563</v>
-      </c>
-      <c r="D3">
-        <v>531</v>
-      </c>
-      <c r="E3">
-        <v>172</v>
-      </c>
-      <c r="F3">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>111</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>92</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>163</v>
       </c>
-      <c r="E4">
-        <v>86</v>
-      </c>
-      <c r="F4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
-        <f>SUM(B2:B4)</f>
-        <v>1459</v>
-      </c>
-      <c r="C5" s="2">
-        <f t="shared" ref="C5:F5" si="0">SUM(C2:C4)</f>
-        <v>1039</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="0"/>
-        <v>1110</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>466</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" si="0"/>
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <f>B2/$B$5</f>
-        <v>0.37217272104180948</v>
-      </c>
-      <c r="C7">
-        <f>C2/$C$5</f>
-        <v>0.36958614051973049</v>
-      </c>
-      <c r="D7">
-        <f>D2/$D$5</f>
-        <v>0.37477477477477478</v>
-      </c>
-      <c r="E7">
-        <f>E2/$E$5</f>
-        <v>0.44635193133047213</v>
-      </c>
-      <c r="F7">
-        <f>F2/$F$5</f>
-        <v>0.46927374301675978</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <f t="shared" ref="B8:B9" si="1">B3/$B$5</f>
-        <v>0.55174777244688145</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:C9" si="2">C3/$C$5</f>
-        <v>0.54186717998075073</v>
-      </c>
-      <c r="D8">
-        <f t="shared" ref="D8:D9" si="3">D3/$D$5</f>
-        <v>0.47837837837837838</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ref="E8:E9" si="4">E3/$E$5</f>
-        <v>0.36909871244635195</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ref="F8:F9" si="5">F3/$F$5</f>
-        <v>0.31284916201117319</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="1"/>
-        <v>7.6079506511309111E-2</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="2"/>
-        <v>8.8546679499518763E-2</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="3"/>
-        <v>0.14684684684684685</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="4"/>
-        <v>0.18454935622317598</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="5"/>
-        <v>0.21787709497206703</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
+      <c r="E4" t="n">
+        <v>89</v>
+      </c>
+      <c r="F4" t="n">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
geomap area 2 and finer area in area 2
- Largest share in the fine area is still monzogranite, but there are also other types of rocks present --> better than geomaps of the entire large areas
- I think i will do 3-5 smaller areas,especially in area 1 and 2
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_count.xlsx
+++ b/_CLUSTER/groups_count.xlsx
@@ -407,10 +407,10 @@
         <v>416</v>
       </c>
       <c r="E2" t="n">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F2" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3">
@@ -427,7 +427,7 @@
         <v>531</v>
       </c>
       <c r="E3" t="n">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F3" t="n">
         <v>56</v>
@@ -447,10 +447,10 @@
         <v>163</v>
       </c>
       <c r="E4" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F4" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>